<commit_message>
complete all the functionalities
</commit_message>
<xml_diff>
--- a/production.xlsx
+++ b/production.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -457,378 +457,219 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-08-01</v>
+        <v>2025-08-30</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>880</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L2">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="M2">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="N2">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="O2">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="P2">
-        <v>14</v>
+        <v>200</v>
       </c>
       <c r="Q2">
-        <v>5</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-31</v>
       </c>
       <c r="B3">
-        <v>909090</v>
+        <v>90</v>
       </c>
       <c r="C3">
-        <v>90</v>
+        <v>800</v>
       </c>
       <c r="D3">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="F3">
-        <v>909</v>
+        <v>80</v>
       </c>
       <c r="G3">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H3">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="I3">
-        <v>909</v>
+        <v>78</v>
       </c>
       <c r="J3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>909</v>
+        <v>98</v>
       </c>
       <c r="L3">
-        <v>910089</v>
+        <v>240</v>
       </c>
       <c r="M3">
-        <v>100000</v>
+        <v>239</v>
       </c>
       <c r="N3">
-        <v>99</v>
+        <v>6865</v>
       </c>
       <c r="O3">
-        <v>1818</v>
+        <v>176</v>
       </c>
       <c r="P3">
-        <v>910188</v>
+        <v>7105</v>
       </c>
       <c r="Q3">
-        <v>101818</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-08-03</v>
+        <v>2025-07-01</v>
       </c>
       <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>90</v>
       </c>
-      <c r="C4">
-        <v>9009</v>
-      </c>
       <c r="D4">
-        <v>909</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>90</v>
+        <v>124529</v>
       </c>
       <c r="F4">
-        <v>9090</v>
+        <v>9</v>
       </c>
       <c r="G4">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="H4">
-        <v>909</v>
+        <v>9</v>
       </c>
       <c r="I4">
         <v>9</v>
       </c>
       <c r="J4">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="K4">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="L4">
-        <v>10089</v>
+        <v>27</v>
       </c>
       <c r="M4">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="N4">
-        <v>999</v>
+        <v>9</v>
       </c>
       <c r="O4">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="P4">
-        <v>11088</v>
+        <v>36</v>
       </c>
       <c r="Q4">
-        <v>189</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-08-04</v>
+        <v>2025-09-01</v>
       </c>
       <c r="B5">
-        <v>9090</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>909</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
       <c r="E5">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="H5">
-        <v>909</v>
+        <v>9</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J5">
-        <v>909</v>
+        <v>9</v>
       </c>
       <c r="K5">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="L5">
-        <v>9189</v>
+        <v>27</v>
       </c>
       <c r="M5">
-        <v>1089</v>
+        <v>27</v>
       </c>
       <c r="N5">
-        <v>1818</v>
+        <v>18</v>
       </c>
       <c r="O5">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="P5">
-        <v>11007</v>
+        <v>45</v>
       </c>
       <c r="Q5">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2025-08-14</v>
-      </c>
-      <c r="B6">
-        <v>99990</v>
-      </c>
-      <c r="C6">
-        <v>87788</v>
-      </c>
-      <c r="D6">
-        <v>787887</v>
-      </c>
-      <c r="E6">
-        <v>87887</v>
-      </c>
-      <c r="F6">
-        <v>78787</v>
-      </c>
-      <c r="G6">
-        <v>787878</v>
-      </c>
-      <c r="H6">
-        <v>8777</v>
-      </c>
-      <c r="I6">
-        <v>8787</v>
-      </c>
-      <c r="J6">
-        <v>78</v>
-      </c>
-      <c r="K6">
-        <v>7878</v>
-      </c>
-      <c r="L6">
-        <v>966664</v>
-      </c>
-      <c r="M6">
-        <v>963553</v>
-      </c>
-      <c r="N6">
-        <v>8855</v>
-      </c>
-      <c r="O6">
-        <v>16665</v>
-      </c>
-      <c r="P6">
-        <v>975519</v>
-      </c>
-      <c r="Q6">
-        <v>980218</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2025-08-28</v>
-      </c>
-      <c r="B7">
-        <v>7877</v>
-      </c>
-      <c r="C7">
-        <v>8787</v>
-      </c>
-      <c r="D7">
-        <v>787</v>
-      </c>
-      <c r="E7">
-        <v>8787</v>
-      </c>
-      <c r="F7">
-        <v>87</v>
-      </c>
-      <c r="G7">
-        <v>878</v>
-      </c>
-      <c r="H7">
-        <v>7877</v>
-      </c>
-      <c r="I7">
-        <v>887</v>
-      </c>
-      <c r="J7">
-        <v>878</v>
-      </c>
-      <c r="K7">
-        <v>78</v>
-      </c>
-      <c r="L7">
-        <v>8751</v>
-      </c>
-      <c r="M7">
-        <v>18452</v>
-      </c>
-      <c r="N7">
-        <v>8755</v>
-      </c>
-      <c r="O7">
-        <v>965</v>
-      </c>
-      <c r="P7">
-        <v>17506</v>
-      </c>
-      <c r="Q7">
-        <v>19417</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>2025-08-29</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>